<commit_message>
Reschedule Loan - Term and Interest change added
</commit_message>
<xml_diff>
--- a/Test_Automation/src/TestData/TestData.xlsx
+++ b/Test_Automation/src/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="5100" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="2790" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="LoanAction" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M11"/>
+  <oleSize ref="A1:O7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -815,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,6 +1130,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reschedule Validations Update and Completion
</commit_message>
<xml_diff>
--- a/Test_Automation/src/TestData/TestData.xlsx
+++ b/Test_Automation/src/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="2790" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="5100" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Flat</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2/10/2014</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -327,6 +333,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1105,34 +1112,43 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>